<commit_message>
add Link Trafo option
</commit_message>
<xml_diff>
--- a/data/Two_Node_Link/Power_Links.xlsx
+++ b/data/Two_Node_Link/Power_Links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Single_Node_Link\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\Two_Node_Link\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2752FF-A3AB-4FB8-BA0D-FC5215595D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1056F686-DB08-4EC9-8708-84CC47BC1D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Format:</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>Node_2</t>
+  </si>
+  <si>
+    <t>Expansion  Trafo</t>
+  </si>
+  <si>
+    <t>pExpTrafoP</t>
+  </si>
+  <si>
+    <t>Additional Link Power with one additional Trafo</t>
   </si>
 </sst>
 </file>
@@ -660,13 +669,13 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,9 +683,10 @@
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>29</v>
@@ -686,8 +696,9 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -695,7 +706,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -717,8 +728,11 @@
       <c r="G3" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -740,8 +754,11 @@
       <c r="G4" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="H4" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>12</v>
@@ -761,8 +778,11 @@
       <c r="G5" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="H5" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
         <v>17</v>
@@ -782,8 +802,11 @@
       <c r="G6" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="H6" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>20</v>
@@ -803,8 +826,11 @@
       <c r="G7" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="H7" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
@@ -822,8 +848,11 @@
       <c r="G8" s="13">
         <v>10000</v>
       </c>
+      <c r="H8" s="13">
+        <v>50</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
@@ -840,6 +869,9 @@
       </c>
       <c r="G9" s="13">
         <v>10000</v>
+      </c>
+      <c r="H9" s="13">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>